<commit_message>
Done with all idivudial modules
</commit_message>
<xml_diff>
--- a/Dashboard/test.xlsx
+++ b/Dashboard/test.xlsx
@@ -14,18 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Pullin' Freight, LLC</t>
   </si>
   <si>
-    <t>Billed to:</t>
-  </si>
-  <si>
-    <t>Address:</t>
-  </si>
-  <si>
-    <t>Invoice from: 2016-11-11 to: 2018-11-11</t>
+    <t>Driver Log For:  Max</t>
+  </si>
+  <si>
+    <t>Rate:</t>
+  </si>
+  <si>
+    <t>Log from: 2015-11-12 to: 2018-11-12</t>
   </si>
   <si>
     <t>Date</t>
@@ -43,25 +43,16 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>Loads/Hours</t>
-  </si>
-  <si>
-    <t>Rate</t>
+    <t>Hours</t>
   </si>
   <si>
     <t>Sub-Total</t>
   </si>
   <si>
-    <t>-8.0% Broker Fee</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>2018-03-25</t>
-  </si>
-  <si>
-    <t>22323113</t>
+    <t>2018-05-12</t>
+  </si>
+  <si>
+    <t>1234567</t>
   </si>
   <si>
     <t>Max Nikias</t>
@@ -70,18 +61,6 @@
     <t>LAX</t>
   </si>
   <si>
-    <t>Lorenzo</t>
-  </si>
-  <si>
-    <t>2018-04-26</t>
-  </si>
-  <si>
-    <t>2018-05-12</t>
-  </si>
-  <si>
-    <t>1234567</t>
-  </si>
-  <si>
     <t>USC</t>
   </si>
   <si>
@@ -95,9 +74,6 @@
   </si>
   <si>
     <t>Grand Total:</t>
-  </si>
-  <si>
-    <t>Submitted: 2018-11-11 by Aarav</t>
   </si>
 </sst>
 </file>
@@ -105,6 +81,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$0.00"/>
     <numFmt numFmtId="164" formatCode="$0.00"/>
     <numFmt numFmtId="164" formatCode="$0.00"/>
     <numFmt numFmtId="164" formatCode="$0.00"/>
@@ -202,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -213,6 +190,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -516,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -547,246 +525,132 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="F5" s="6">
+        <v>5</v>
+      </c>
+      <c r="G5" s="7">
+        <f>B3*F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8">
+        <v>5</v>
+      </c>
+      <c r="G6" s="9">
+        <f>B3*F6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5">
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="6">
         <v>5</v>
       </c>
-      <c r="G5" s="6">
-        <v>12</v>
-      </c>
-      <c r="H5" s="6">
-        <f>F5*G5</f>
+      <c r="G7" s="7">
+        <f>B3*F7</f>
         <v>0</v>
       </c>
-      <c r="I5" s="6">
-        <f>H5*0.08</f>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="D8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F5:F7)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="6">
-        <f>H5-I5</f>
+      <c r="G8" s="10">
+        <f>SUM(G5:G7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7">
-        <v>5</v>
-      </c>
-      <c r="G6" s="8">
-        <v>12</v>
-      </c>
-      <c r="H6" s="8">
-        <f>F6*G6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <f>H6*0.08</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="8">
-        <f>H6-I6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="5">
-        <v>5</v>
-      </c>
-      <c r="G7" s="6">
-        <v>12</v>
-      </c>
-      <c r="H7" s="6">
-        <f>F7*G7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <f>H7*0.08</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <f>H7-I7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="7">
-        <v>5</v>
-      </c>
-      <c r="G8" s="8">
-        <v>12</v>
-      </c>
-      <c r="H8" s="8">
-        <f>F8*G8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <f>H8*0.08</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="8">
-        <f>H8-I8</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="5">
-        <v>5</v>
-      </c>
-      <c r="G9" s="6">
-        <v>12</v>
-      </c>
-      <c r="H9" s="6">
-        <f>F9*G9</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <f>H9*0.08</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <f>H9-I9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="I10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="9">
-        <f>SUM(J5:J9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>